<commit_message>
[FEATURE] agregar los mismos campos al importar que en el formulario
</commit_message>
<xml_diff>
--- a/public/downloads/template-clientes.xlsx
+++ b/public/downloads/template-clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hugger\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A8DB78-D093-4DE0-8E51-52D42B4A93DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB1C47-ED4B-4AE3-8A7B-19BE4DC6DB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F9635639-F99E-4782-9988-7D00D6FB64B1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F9635639-F99E-4782-9988-7D00D6FB64B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Nombre</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Fuente</t>
   </si>
   <si>
-    <t>Medio</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -92,21 +89,6 @@
     <t>Eventos</t>
   </si>
   <si>
-    <t>TELÉFONO</t>
-  </si>
-  <si>
-    <t>WHATSAPP</t>
-  </si>
-  <si>
-    <t>CORREO</t>
-  </si>
-  <si>
-    <t>FORMULARIO PÁGINA WEB</t>
-  </si>
-  <si>
-    <t>REDES</t>
-  </si>
-  <si>
     <t>Persona Natural 2</t>
   </si>
   <si>
@@ -192,13 +174,31 @@
   </si>
   <si>
     <t>aliado1-contacto2@wishy.fr</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Avenida Siempre Viva 123</t>
+  </si>
+  <si>
+    <t>Envigado</t>
+  </si>
+  <si>
+    <t>Jhonatan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +228,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,13 +309,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAB255B-47FF-4073-85C2-952A506FD25C}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,15 +665,16 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="7" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -672,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -681,279 +691,271 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111111</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2">
         <v>456789</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>111112</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>111113</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>111114</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>111115</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>111116</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>222221</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D8">
         <v>987654</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8">
         <v>444441</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9">
+      <c r="L8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9">
         <v>444442</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10">
+      <c r="L9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10">
         <v>444443</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>222222</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11">
+      <c r="K11">
         <v>444444</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>222222</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
         <v>444445</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>222222</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="6"/>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>333331</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14">
         <v>444446</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>